<commit_message>
finished up lcgov data wrangling and added documentation as well as tests
</commit_message>
<xml_diff>
--- a/inst/extdata/additional_govdata.xlsx
+++ b/inst/extdata/additional_govdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Git_Projekte\bundeslaendeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7447CBA0-962F-4184-88F5-66C128A43CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CD8487-3AE3-42B7-9799-ADDED4E3A98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -261,9 +261,6 @@
     <t>1948-01-22</t>
   </si>
   <si>
-    <t>KPD</t>
-  </si>
-  <si>
     <t>1947-03-27</t>
   </si>
   <si>
@@ -727,6 +724,9 @@
   </si>
   <si>
     <t>https://de.wikipedia.org/wiki/Regierungskrise_in_Th%C3%BCringen_2020#F%C3%BChrung_der_Regierungsgesch%C3%A4fte</t>
+  </si>
+  <si>
+    <t>KPD (1919)</t>
   </si>
 </sst>
 </file>
@@ -1049,8 +1049,8 @@
   <dimension ref="A1:I218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E225" sqref="E225"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1090,7 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2284,7 +2284,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>10430</v>
+        <v>10431</v>
       </c>
       <c r="B43" t="s">
         <v>40</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>10430</v>
+        <v>10431</v>
       </c>
       <c r="B44" t="s">
         <v>40</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>10431</v>
+        <v>10432</v>
       </c>
       <c r="B45" t="s">
         <v>40</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>10431</v>
+        <v>10432</v>
       </c>
       <c r="B46" t="s">
         <v>40</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>10431</v>
+        <v>10432</v>
       </c>
       <c r="B47" t="s">
         <v>40</v>
@@ -2763,7 +2763,7 @@
         <v>73</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G59" t="s">
         <v>20</v>
@@ -2792,7 +2792,7 @@
         <v>73</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G60" t="s">
         <v>11</v>
@@ -2821,10 +2821,10 @@
         <v>73</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G61" t="s">
-        <v>75</v>
+        <v>230</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -2847,7 +2847,7 @@
         <v>0</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>74</v>
@@ -2876,7 +2876,7 @@
         <v>0</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>74</v>
@@ -2905,10 +2905,10 @@
         <v>19</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="G64" t="s">
         <v>10</v>
@@ -2934,10 +2934,10 @@
         <v>19</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="G65" t="s">
         <v>20</v>
@@ -2963,10 +2963,10 @@
         <v>20</v>
       </c>
       <c r="E66" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="G66" t="s">
         <v>10</v>
@@ -2975,7 +2975,7 @@
         <v>4</v>
       </c>
       <c r="I66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2992,10 +2992,10 @@
         <v>20</v>
       </c>
       <c r="E67" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="G67" t="s">
         <v>20</v>
@@ -3004,7 +3004,7 @@
         <v>3</v>
       </c>
       <c r="I67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3021,10 +3021,10 @@
         <v>21</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G68" t="s">
         <v>20</v>
@@ -3033,7 +3033,7 @@
         <v>6</v>
       </c>
       <c r="I68" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3050,10 +3050,10 @@
         <v>21</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G69" t="s">
         <v>18</v>
@@ -3062,7 +3062,7 @@
         <v>2</v>
       </c>
       <c r="I69" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3079,10 +3079,10 @@
         <v>22</v>
       </c>
       <c r="E70" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="G70" t="s">
         <v>20</v>
@@ -3091,7 +3091,7 @@
         <v>5</v>
       </c>
       <c r="I70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3108,10 +3108,10 @@
         <v>22</v>
       </c>
       <c r="E71" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F71" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="G71" t="s">
         <v>18</v>
@@ -3120,7 +3120,7 @@
         <v>3</v>
       </c>
       <c r="I71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3137,10 +3137,10 @@
         <v>23</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G72" t="s">
         <v>20</v>
@@ -3149,7 +3149,7 @@
         <v>6</v>
       </c>
       <c r="I72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3166,10 +3166,10 @@
         <v>23</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G73" t="s">
         <v>18</v>
@@ -3178,7 +3178,7 @@
         <v>3</v>
       </c>
       <c r="I73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3195,7 +3195,7 @@
         <v>24</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>24</v>
@@ -3207,7 +3207,7 @@
         <v>4</v>
       </c>
       <c r="I74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3224,7 +3224,7 @@
         <v>24</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>24</v>
@@ -3236,7 +3236,7 @@
         <v>3</v>
       </c>
       <c r="I75" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3253,7 +3253,7 @@
         <v>24</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>24</v>
@@ -3265,7 +3265,7 @@
         <v>2</v>
       </c>
       <c r="I76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3273,7 +3273,7 @@
         <v>10720</v>
       </c>
       <c r="B77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C77">
         <v>16</v>
@@ -3282,10 +3282,10 @@
         <v>20</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G77" t="s">
         <v>10</v>
@@ -3302,7 +3302,7 @@
         <v>10721</v>
       </c>
       <c r="B78" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C78">
         <v>17</v>
@@ -3311,10 +3311,10 @@
         <v>21</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G78" t="s">
         <v>10</v>
@@ -3323,7 +3323,7 @@
         <v>9</v>
       </c>
       <c r="I78" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3331,7 +3331,7 @@
         <v>10722</v>
       </c>
       <c r="B79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C79">
         <v>18</v>
@@ -3340,10 +3340,10 @@
         <v>22</v>
       </c>
       <c r="E79" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="G79" t="s">
         <v>10</v>
@@ -3352,7 +3352,7 @@
         <v>8</v>
       </c>
       <c r="I79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3360,7 +3360,7 @@
         <v>10722</v>
       </c>
       <c r="B80" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C80">
         <v>18</v>
@@ -3369,10 +3369,10 @@
         <v>22</v>
       </c>
       <c r="E80" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="G80" t="s">
         <v>11</v>
@@ -3381,7 +3381,7 @@
         <v>4</v>
       </c>
       <c r="I80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3389,7 +3389,7 @@
         <v>10723</v>
       </c>
       <c r="B81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C81">
         <v>18</v>
@@ -3398,10 +3398,10 @@
         <v>23</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G81" t="s">
         <v>10</v>
@@ -3410,7 +3410,7 @@
         <v>8</v>
       </c>
       <c r="I81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3418,7 +3418,7 @@
         <v>10723</v>
       </c>
       <c r="B82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C82">
         <v>18</v>
@@ -3427,10 +3427,10 @@
         <v>23</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G82" t="s">
         <v>11</v>
@@ -3439,7 +3439,7 @@
         <v>4</v>
       </c>
       <c r="I82" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3447,7 +3447,7 @@
         <v>10724</v>
       </c>
       <c r="B83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C83">
         <v>19</v>
@@ -3456,10 +3456,10 @@
         <v>24</v>
       </c>
       <c r="E83" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="G83" t="s">
         <v>10</v>
@@ -3468,7 +3468,7 @@
         <v>9</v>
       </c>
       <c r="I83" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3476,7 +3476,7 @@
         <v>10724</v>
       </c>
       <c r="B84" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C84">
         <v>19</v>
@@ -3485,10 +3485,10 @@
         <v>24</v>
       </c>
       <c r="E84" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="G84" t="s">
         <v>18</v>
@@ -3497,7 +3497,7 @@
         <v>2</v>
       </c>
       <c r="I84" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -3505,7 +3505,7 @@
         <v>10725</v>
       </c>
       <c r="B85" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C85">
         <v>20</v>
@@ -3514,7 +3514,7 @@
         <v>25</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>24</v>
@@ -3526,7 +3526,7 @@
         <v>8</v>
       </c>
       <c r="I85" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
         <v>10725</v>
       </c>
       <c r="B86" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C86">
         <v>20</v>
@@ -3543,7 +3543,7 @@
         <v>25</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>24</v>
@@ -3555,7 +3555,7 @@
         <v>4</v>
       </c>
       <c r="I86" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3563,7 +3563,7 @@
         <v>10826</v>
       </c>
       <c r="B87" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C87">
         <v>18</v>
@@ -3572,10 +3572,10 @@
         <v>26</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G87" t="s">
         <v>10</v>
@@ -3592,7 +3592,7 @@
         <v>10827</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C88">
         <v>19</v>
@@ -3601,10 +3601,10 @@
         <v>27</v>
       </c>
       <c r="E88" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="G88" t="s">
         <v>10</v>
@@ -3613,7 +3613,7 @@
         <v>6</v>
       </c>
       <c r="I88" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -3621,7 +3621,7 @@
         <v>10827</v>
       </c>
       <c r="B89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C89">
         <v>19</v>
@@ -3630,10 +3630,10 @@
         <v>27</v>
       </c>
       <c r="E89" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F89" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="G89" t="s">
         <v>18</v>
@@ -3642,7 +3642,7 @@
         <v>3</v>
       </c>
       <c r="I89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3650,7 +3650,7 @@
         <v>10828</v>
       </c>
       <c r="B90" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C90">
         <v>19</v>
@@ -3659,10 +3659,10 @@
         <v>28</v>
       </c>
       <c r="E90" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F90" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="G90" t="s">
         <v>10</v>
@@ -3671,7 +3671,7 @@
         <v>8</v>
       </c>
       <c r="I90" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3679,7 +3679,7 @@
         <v>10828</v>
       </c>
       <c r="B91" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C91">
         <v>19</v>
@@ -3688,10 +3688,10 @@
         <v>28</v>
       </c>
       <c r="E91" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F91" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="G91" t="s">
         <v>18</v>
@@ -3700,7 +3700,7 @@
         <v>3</v>
       </c>
       <c r="I91" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3708,7 +3708,7 @@
         <v>10829</v>
       </c>
       <c r="B92" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C92">
         <v>19</v>
@@ -3717,10 +3717,10 @@
         <v>29</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G92" t="s">
         <v>10</v>
@@ -3729,7 +3729,7 @@
         <v>8</v>
       </c>
       <c r="I92" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -3737,7 +3737,7 @@
         <v>10830</v>
       </c>
       <c r="B93" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C93">
         <v>20</v>
@@ -3746,10 +3746,10 @@
         <v>30</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G93" t="s">
         <v>20</v>
@@ -3758,7 +3758,7 @@
         <v>9</v>
       </c>
       <c r="I93" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -3766,7 +3766,7 @@
         <v>10831</v>
       </c>
       <c r="B94" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C94">
         <v>21</v>
@@ -3775,10 +3775,10 @@
         <v>31</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G94" t="s">
         <v>20</v>
@@ -3787,7 +3787,7 @@
         <v>8</v>
       </c>
       <c r="I94" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -3795,7 +3795,7 @@
         <v>10831</v>
       </c>
       <c r="B95" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C95">
         <v>21</v>
@@ -3804,10 +3804,10 @@
         <v>31</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G95" t="s">
         <v>18</v>
@@ -3816,7 +3816,7 @@
         <v>3</v>
       </c>
       <c r="I95" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -3824,7 +3824,7 @@
         <v>10832</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C96">
         <v>21</v>
@@ -3833,10 +3833,10 @@
         <v>32</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G96" t="s">
         <v>20</v>
@@ -3845,7 +3845,7 @@
         <v>8</v>
       </c>
       <c r="I96" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -3853,7 +3853,7 @@
         <v>10832</v>
       </c>
       <c r="B97" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C97">
         <v>21</v>
@@ -3862,10 +3862,10 @@
         <v>32</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G97" t="s">
         <v>18</v>
@@ -3874,7 +3874,7 @@
         <v>3</v>
       </c>
       <c r="I97" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -3882,7 +3882,7 @@
         <v>10833</v>
       </c>
       <c r="B98" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C98">
         <v>22</v>
@@ -3891,7 +3891,7 @@
         <v>33</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>24</v>
@@ -3903,7 +3903,7 @@
         <v>7</v>
       </c>
       <c r="I98" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -3911,7 +3911,7 @@
         <v>10833</v>
       </c>
       <c r="B99" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C99">
         <v>22</v>
@@ -3920,7 +3920,7 @@
         <v>33</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>24</v>
@@ -3932,7 +3932,7 @@
         <v>4</v>
       </c>
       <c r="I99" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -3940,7 +3940,7 @@
         <v>10905</v>
       </c>
       <c r="B100" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C100">
         <v>4</v>
@@ -3949,10 +3949,10 @@
         <v>5</v>
       </c>
       <c r="E100" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="G100" t="s">
         <v>20</v>
@@ -3969,7 +3969,7 @@
         <v>10905</v>
       </c>
       <c r="B101" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C101">
         <v>4</v>
@@ -3978,10 +3978,10 @@
         <v>5</v>
       </c>
       <c r="E101" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F101" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="G101" t="s">
         <v>53</v>
@@ -3998,7 +3998,7 @@
         <v>10906</v>
       </c>
       <c r="B102" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C102">
         <v>5</v>
@@ -4007,10 +4007,10 @@
         <v>6</v>
       </c>
       <c r="E102" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F102" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="G102" t="s">
         <v>20</v>
@@ -4019,7 +4019,7 @@
         <v>5</v>
       </c>
       <c r="I102" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4027,7 +4027,7 @@
         <v>10906</v>
       </c>
       <c r="B103" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C103">
         <v>5</v>
@@ -4036,10 +4036,10 @@
         <v>6</v>
       </c>
       <c r="E103" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F103" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="G103" t="s">
         <v>10</v>
@@ -4048,7 +4048,7 @@
         <v>4</v>
       </c>
       <c r="I103" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4056,7 +4056,7 @@
         <v>10910</v>
       </c>
       <c r="B104" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C104">
         <v>5</v>
@@ -4065,10 +4065,10 @@
         <v>7</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G104" t="s">
         <v>20</v>
@@ -4077,7 +4077,7 @@
         <v>5</v>
       </c>
       <c r="I104" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4085,7 +4085,7 @@
         <v>10910</v>
       </c>
       <c r="B105" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C105">
         <v>5</v>
@@ -4094,10 +4094,10 @@
         <v>7</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G105" t="s">
         <v>10</v>
@@ -4106,7 +4106,7 @@
         <v>4</v>
       </c>
       <c r="I105" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4114,7 +4114,7 @@
         <v>10911</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C106">
         <v>6</v>
@@ -4123,10 +4123,10 @@
         <v>8</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G106" t="s">
         <v>20</v>
@@ -4135,7 +4135,7 @@
         <v>6</v>
       </c>
       <c r="I106" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -4143,7 +4143,7 @@
         <v>10911</v>
       </c>
       <c r="B107" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C107">
         <v>6</v>
@@ -4152,10 +4152,10 @@
         <v>8</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G107" t="s">
         <v>10</v>
@@ -4164,7 +4164,7 @@
         <v>3</v>
       </c>
       <c r="I107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4172,7 +4172,7 @@
         <v>10912</v>
       </c>
       <c r="B108" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C108">
         <v>7</v>
@@ -4181,10 +4181,10 @@
         <v>9</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G108" t="s">
         <v>20</v>
@@ -4193,7 +4193,7 @@
         <v>6</v>
       </c>
       <c r="I108" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4201,7 +4201,7 @@
         <v>10912</v>
       </c>
       <c r="B109" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C109">
         <v>7</v>
@@ -4210,10 +4210,10 @@
         <v>9</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G109" t="s">
         <v>10</v>
@@ -4222,7 +4222,7 @@
         <v>3</v>
       </c>
       <c r="I109" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4230,7 +4230,7 @@
         <v>10913</v>
       </c>
       <c r="B110" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C110">
         <v>7</v>
@@ -4239,7 +4239,7 @@
         <v>10</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>24</v>
@@ -4251,7 +4251,7 @@
         <v>6</v>
       </c>
       <c r="I110" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4259,7 +4259,7 @@
         <v>10913</v>
       </c>
       <c r="B111" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C111">
         <v>7</v>
@@ -4268,7 +4268,7 @@
         <v>10</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>24</v>
@@ -4280,7 +4280,7 @@
         <v>3</v>
       </c>
       <c r="I111" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4288,7 +4288,7 @@
         <v>11027</v>
       </c>
       <c r="B112" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C112">
         <v>15</v>
@@ -4297,10 +4297,10 @@
         <v>27</v>
       </c>
       <c r="E112" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F112" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="G112" t="s">
         <v>10</v>
@@ -4317,7 +4317,7 @@
         <v>11027</v>
       </c>
       <c r="B113" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C113">
         <v>15</v>
@@ -4326,10 +4326,10 @@
         <v>27</v>
       </c>
       <c r="E113" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F113" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="G113" t="s">
         <v>11</v>
@@ -4346,7 +4346,7 @@
         <v>11028</v>
       </c>
       <c r="B114" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C114">
         <v>16</v>
@@ -4355,10 +4355,10 @@
         <v>28</v>
       </c>
       <c r="E114" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F114" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="G114" t="s">
         <v>10</v>
@@ -4367,7 +4367,7 @@
         <v>8</v>
       </c>
       <c r="I114" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -4375,7 +4375,7 @@
         <v>11028</v>
       </c>
       <c r="B115" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C115">
         <v>16</v>
@@ -4384,10 +4384,10 @@
         <v>28</v>
       </c>
       <c r="E115" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F115" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="G115" t="s">
         <v>11</v>
@@ -4396,7 +4396,7 @@
         <v>3</v>
       </c>
       <c r="I115" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -4404,7 +4404,7 @@
         <v>11029</v>
       </c>
       <c r="B116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C116">
         <v>16</v>
@@ -4413,10 +4413,10 @@
         <v>29</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G116" t="s">
         <v>10</v>
@@ -4425,7 +4425,7 @@
         <v>8</v>
       </c>
       <c r="I116" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4433,7 +4433,7 @@
         <v>11029</v>
       </c>
       <c r="B117" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C117">
         <v>16</v>
@@ -4442,10 +4442,10 @@
         <v>29</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G117" t="s">
         <v>11</v>
@@ -4454,7 +4454,7 @@
         <v>3</v>
       </c>
       <c r="I117" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -4462,7 +4462,7 @@
         <v>11030</v>
       </c>
       <c r="B118" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C118">
         <v>17</v>
@@ -4471,10 +4471,10 @@
         <v>30</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G118" t="s">
         <v>20</v>
@@ -4483,7 +4483,7 @@
         <v>6</v>
       </c>
       <c r="I118" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -4491,7 +4491,7 @@
         <v>11030</v>
       </c>
       <c r="B119" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C119">
         <v>17</v>
@@ -4500,10 +4500,10 @@
         <v>30</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G119" t="s">
         <v>18</v>
@@ -4512,7 +4512,7 @@
         <v>4</v>
       </c>
       <c r="I119" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -4520,7 +4520,7 @@
         <v>11031</v>
       </c>
       <c r="B120" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C120">
         <v>18</v>
@@ -4529,7 +4529,7 @@
         <v>31</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>24</v>
@@ -4541,7 +4541,7 @@
         <v>6</v>
       </c>
       <c r="I120" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -4549,7 +4549,7 @@
         <v>11031</v>
       </c>
       <c r="B121" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C121">
         <v>18</v>
@@ -4558,7 +4558,7 @@
         <v>31</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>24</v>
@@ -4570,7 +4570,7 @@
         <v>5</v>
       </c>
       <c r="I121" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -4578,7 +4578,7 @@
         <v>11122</v>
       </c>
       <c r="B122" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C122">
         <v>14</v>
@@ -4587,10 +4587,10 @@
         <v>22</v>
       </c>
       <c r="E122" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F122" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="G122" t="s">
         <v>10</v>
@@ -4607,7 +4607,7 @@
         <v>11122</v>
       </c>
       <c r="B123" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C123">
         <v>14</v>
@@ -4616,10 +4616,10 @@
         <v>22</v>
       </c>
       <c r="E123" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F123" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="G123" t="s">
         <v>11</v>
@@ -4636,7 +4636,7 @@
         <v>11123</v>
       </c>
       <c r="B124" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C124">
         <v>15</v>
@@ -4645,10 +4645,10 @@
         <v>23</v>
       </c>
       <c r="E124" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F124" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="G124" t="s">
         <v>20</v>
@@ -4657,7 +4657,7 @@
         <v>9</v>
       </c>
       <c r="I124" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -4665,7 +4665,7 @@
         <v>11123</v>
       </c>
       <c r="B125" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C125">
         <v>15</v>
@@ -4674,10 +4674,10 @@
         <v>23</v>
       </c>
       <c r="E125" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F125" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="G125" t="s">
         <v>18</v>
@@ -4686,7 +4686,7 @@
         <v>2</v>
       </c>
       <c r="I125" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -4694,7 +4694,7 @@
         <v>11124</v>
       </c>
       <c r="B126" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C126">
         <v>16</v>
@@ -4703,10 +4703,10 @@
         <v>24</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G126" t="s">
         <v>20</v>
@@ -4715,7 +4715,7 @@
         <v>10</v>
       </c>
       <c r="I126" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -4723,7 +4723,7 @@
         <v>11124</v>
       </c>
       <c r="B127" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C127">
         <v>16</v>
@@ -4732,10 +4732,10 @@
         <v>24</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G127" t="s">
         <v>18</v>
@@ -4744,7 +4744,7 @@
         <v>3</v>
       </c>
       <c r="I127" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -4752,7 +4752,7 @@
         <v>11125</v>
       </c>
       <c r="B128" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C128">
         <v>17</v>
@@ -4761,7 +4761,7 @@
         <v>25</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>24</v>
@@ -4773,7 +4773,7 @@
         <v>10</v>
       </c>
       <c r="I128" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -4781,7 +4781,7 @@
         <v>11125</v>
       </c>
       <c r="B129" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C129">
         <v>17</v>
@@ -4790,7 +4790,7 @@
         <v>25</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>24</v>
@@ -4802,7 +4802,7 @@
         <v>3</v>
       </c>
       <c r="I129" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -4810,7 +4810,7 @@
         <v>11221</v>
       </c>
       <c r="B130" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C130">
         <v>14</v>
@@ -4819,10 +4819,10 @@
         <v>21</v>
       </c>
       <c r="E130" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F130" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="G130" t="s">
         <v>10</v>
@@ -4839,7 +4839,7 @@
         <v>11221</v>
       </c>
       <c r="B131" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C131">
         <v>14</v>
@@ -4848,10 +4848,10 @@
         <v>21</v>
       </c>
       <c r="E131" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F131" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="G131" t="s">
         <v>20</v>
@@ -4868,7 +4868,7 @@
         <v>11222</v>
       </c>
       <c r="B132" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C132">
         <v>15</v>
@@ -4877,10 +4877,10 @@
         <v>22</v>
       </c>
       <c r="E132" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F132" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G132" t="s">
         <v>20</v>
@@ -4889,7 +4889,7 @@
         <v>10</v>
       </c>
       <c r="I132" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -4897,7 +4897,7 @@
         <v>11223</v>
       </c>
       <c r="B133" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C133">
         <v>16</v>
@@ -4906,10 +4906,10 @@
         <v>23</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G133" t="s">
         <v>20</v>
@@ -4918,7 +4918,7 @@
         <v>7</v>
       </c>
       <c r="I133" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -4926,7 +4926,7 @@
         <v>11223</v>
       </c>
       <c r="B134" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C134">
         <v>16</v>
@@ -4935,10 +4935,10 @@
         <v>23</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G134" t="s">
         <v>18</v>
@@ -4947,7 +4947,7 @@
         <v>3</v>
       </c>
       <c r="I134" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -4955,7 +4955,7 @@
         <v>11224</v>
       </c>
       <c r="B135" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C135">
         <v>16</v>
@@ -4964,10 +4964,10 @@
         <v>24</v>
       </c>
       <c r="E135" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F135" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="G135" t="s">
         <v>20</v>
@@ -4976,7 +4976,7 @@
         <v>7</v>
       </c>
       <c r="I135" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -4984,7 +4984,7 @@
         <v>11224</v>
       </c>
       <c r="B136" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C136">
         <v>16</v>
@@ -4993,10 +4993,10 @@
         <v>24</v>
       </c>
       <c r="E136" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F136" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="G136" t="s">
         <v>18</v>
@@ -5005,7 +5005,7 @@
         <v>3</v>
       </c>
       <c r="I136" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -5013,7 +5013,7 @@
         <v>11225</v>
       </c>
       <c r="B137" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C137">
         <v>17</v>
@@ -5022,10 +5022,10 @@
         <v>25</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G137" t="s">
         <v>20</v>
@@ -5034,7 +5034,7 @@
         <v>6</v>
       </c>
       <c r="I137" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -5042,7 +5042,7 @@
         <v>11225</v>
       </c>
       <c r="B138" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C138">
         <v>17</v>
@@ -5051,10 +5051,10 @@
         <v>25</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G138" t="s">
         <v>11</v>
@@ -5063,7 +5063,7 @@
         <v>2</v>
       </c>
       <c r="I138" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -5071,7 +5071,7 @@
         <v>11225</v>
       </c>
       <c r="B139" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C139">
         <v>17</v>
@@ -5080,10 +5080,10 @@
         <v>25</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G139" t="s">
         <v>18</v>
@@ -5092,7 +5092,7 @@
         <v>2</v>
       </c>
       <c r="I139" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -5100,7 +5100,7 @@
         <v>11226</v>
       </c>
       <c r="B140" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C140">
         <v>18</v>
@@ -5109,7 +5109,7 @@
         <v>26</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>24</v>
@@ -5121,7 +5121,7 @@
         <v>6</v>
       </c>
       <c r="I140" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -5129,7 +5129,7 @@
         <v>11226</v>
       </c>
       <c r="B141" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C141">
         <v>18</v>
@@ -5138,7 +5138,7 @@
         <v>26</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>24</v>
@@ -5150,7 +5150,7 @@
         <v>2</v>
       </c>
       <c r="I141" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -5158,7 +5158,7 @@
         <v>11226</v>
       </c>
       <c r="B142" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C142">
         <v>18</v>
@@ -5167,7 +5167,7 @@
         <v>26</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>24</v>
@@ -5179,7 +5179,7 @@
         <v>2</v>
       </c>
       <c r="I142" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -5187,7 +5187,7 @@
         <v>11314</v>
       </c>
       <c r="B143" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C143">
         <v>-2</v>
@@ -5196,19 +5196,19 @@
         <v>-9</v>
       </c>
       <c r="E143" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F143" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F143" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="G143" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H143">
         <v>4</v>
       </c>
       <c r="I143" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -5216,7 +5216,7 @@
         <v>11314</v>
       </c>
       <c r="B144" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C144">
         <v>-2</v>
@@ -5225,19 +5225,19 @@
         <v>-9</v>
       </c>
       <c r="E144" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F144" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F144" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="G144" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H144">
         <v>2</v>
       </c>
       <c r="I144" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -5245,7 +5245,7 @@
         <v>11315</v>
       </c>
       <c r="B145" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C145">
         <v>-2</v>
@@ -5254,19 +5254,19 @@
         <v>-8</v>
       </c>
       <c r="E145" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F145" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F145" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="G145" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H145">
         <v>5</v>
       </c>
       <c r="I145" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -5274,7 +5274,7 @@
         <v>11316</v>
       </c>
       <c r="B146" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C146">
         <v>-1</v>
@@ -5283,19 +5283,19 @@
         <v>-7</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G146" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H146">
         <v>7</v>
       </c>
       <c r="I146" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -5303,7 +5303,7 @@
         <v>11316</v>
       </c>
       <c r="B147" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C147">
         <v>-1</v>
@@ -5312,19 +5312,19 @@
         <v>-7</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G147" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H147">
         <v>2</v>
       </c>
       <c r="I147" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -5332,7 +5332,7 @@
         <v>11317</v>
       </c>
       <c r="B148" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C148">
         <v>-1</v>
@@ -5341,19 +5341,19 @@
         <v>-6</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G148" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H148">
         <v>6</v>
       </c>
       <c r="I148" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -5361,7 +5361,7 @@
         <v>11318</v>
       </c>
       <c r="B149" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C149">
         <v>-1</v>
@@ -5370,19 +5370,19 @@
         <v>-5</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F149" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G149" t="s">
         <v>170</v>
-      </c>
-      <c r="G149" t="s">
-        <v>171</v>
       </c>
       <c r="H149">
         <v>6</v>
       </c>
       <c r="I149" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -5390,7 +5390,7 @@
         <v>11319</v>
       </c>
       <c r="B150" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -5399,10 +5399,10 @@
         <v>-4</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G150" t="s">
         <v>10</v>
@@ -5411,7 +5411,7 @@
         <v>4</v>
       </c>
       <c r="I150" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -5419,7 +5419,7 @@
         <v>11319</v>
       </c>
       <c r="B151" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -5428,10 +5428,10 @@
         <v>-4</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G151" t="s">
         <v>20</v>
@@ -5440,7 +5440,7 @@
         <v>1</v>
       </c>
       <c r="I151" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -5448,7 +5448,7 @@
         <v>11319</v>
       </c>
       <c r="B152" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -5457,10 +5457,10 @@
         <v>-4</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G152" t="s">
         <v>11</v>
@@ -5469,7 +5469,7 @@
         <v>1</v>
       </c>
       <c r="I152" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -5477,7 +5477,7 @@
         <v>11320</v>
       </c>
       <c r="B153" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -5486,10 +5486,10 @@
         <v>-3</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G153" t="s">
         <v>10</v>
@@ -5498,7 +5498,7 @@
         <v>4</v>
       </c>
       <c r="I153" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -5506,7 +5506,7 @@
         <v>11320</v>
       </c>
       <c r="B154" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -5515,10 +5515,10 @@
         <v>-3</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G154" t="s">
         <v>20</v>
@@ -5527,7 +5527,7 @@
         <v>1</v>
       </c>
       <c r="I154" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -5535,7 +5535,7 @@
         <v>11321</v>
       </c>
       <c r="B155" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -5544,10 +5544,10 @@
         <v>-2</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G155" t="s">
         <v>10</v>
@@ -5556,7 +5556,7 @@
         <v>5</v>
       </c>
       <c r="I155" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -5564,7 +5564,7 @@
         <v>11321</v>
       </c>
       <c r="B156" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -5573,10 +5573,10 @@
         <v>-2</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G156" t="s">
         <v>20</v>
@@ -5585,7 +5585,7 @@
         <v>1</v>
       </c>
       <c r="I156" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -5593,7 +5593,7 @@
         <v>11321</v>
       </c>
       <c r="B157" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -5602,10 +5602,10 @@
         <v>-2</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G157" t="s">
         <v>11</v>
@@ -5614,7 +5614,7 @@
         <v>2</v>
       </c>
       <c r="I157" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -5622,7 +5622,7 @@
         <v>11322</v>
       </c>
       <c r="B158" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -5631,10 +5631,10 @@
         <v>-1</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G158" t="s">
         <v>10</v>
@@ -5643,7 +5643,7 @@
         <v>4</v>
       </c>
       <c r="I158" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -5651,7 +5651,7 @@
         <v>11322</v>
       </c>
       <c r="B159" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -5660,10 +5660,10 @@
         <v>-1</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G159" t="s">
         <v>20</v>
@@ -5672,7 +5672,7 @@
         <v>2</v>
       </c>
       <c r="I159" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -5680,7 +5680,7 @@
         <v>11322</v>
       </c>
       <c r="B160" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -5689,19 +5689,19 @@
         <v>-1</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G160" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H160">
         <v>1</v>
       </c>
       <c r="I160" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -5709,7 +5709,7 @@
         <v>11323</v>
       </c>
       <c r="B161" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -5718,10 +5718,10 @@
         <v>0</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G161" t="s">
         <v>10</v>
@@ -5730,7 +5730,7 @@
         <v>6</v>
       </c>
       <c r="I161" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -5738,7 +5738,7 @@
         <v>11323</v>
       </c>
       <c r="B162" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -5747,10 +5747,10 @@
         <v>0</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G162" t="s">
         <v>20</v>
@@ -5759,7 +5759,7 @@
         <v>2</v>
       </c>
       <c r="I162" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -5767,7 +5767,7 @@
         <v>11313</v>
       </c>
       <c r="B163" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C163">
         <v>10</v>
@@ -5776,10 +5776,10 @@
         <v>13</v>
       </c>
       <c r="E163" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F163" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="G163" t="s">
         <v>10</v>
@@ -5796,7 +5796,7 @@
         <v>11324</v>
       </c>
       <c r="B164" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C164">
         <v>11</v>
@@ -5805,10 +5805,10 @@
         <v>14</v>
       </c>
       <c r="E164" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F164" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="F164" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="G164" t="s">
         <v>10</v>
@@ -5817,7 +5817,7 @@
         <v>5</v>
       </c>
       <c r="I164" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
@@ -5825,7 +5825,7 @@
         <v>11324</v>
       </c>
       <c r="B165" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C165">
         <v>11</v>
@@ -5834,10 +5834,10 @@
         <v>14</v>
       </c>
       <c r="E165" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F165" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="F165" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="G165" t="s">
         <v>11</v>
@@ -5846,7 +5846,7 @@
         <v>2</v>
       </c>
       <c r="I165" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -5854,7 +5854,7 @@
         <v>11324</v>
       </c>
       <c r="B166" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C166">
         <v>11</v>
@@ -5863,10 +5863,10 @@
         <v>14</v>
       </c>
       <c r="E166" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F166" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="F166" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="G166" t="s">
         <v>18</v>
@@ -5875,7 +5875,7 @@
         <v>2</v>
       </c>
       <c r="I166" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -5883,7 +5883,7 @@
         <v>11325</v>
       </c>
       <c r="B167" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C167">
         <v>11</v>
@@ -5892,10 +5892,10 @@
         <v>15</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G167" t="s">
         <v>10</v>
@@ -5904,7 +5904,7 @@
         <v>5</v>
       </c>
       <c r="I167" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -5912,7 +5912,7 @@
         <v>11325</v>
       </c>
       <c r="B168" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C168">
         <v>11</v>
@@ -5921,10 +5921,10 @@
         <v>15</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G168" t="s">
         <v>11</v>
@@ -5933,7 +5933,7 @@
         <v>2</v>
       </c>
       <c r="I168" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -5941,7 +5941,7 @@
         <v>11325</v>
       </c>
       <c r="B169" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C169">
         <v>11</v>
@@ -5950,10 +5950,10 @@
         <v>15</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G169" t="s">
         <v>18</v>
@@ -5962,7 +5962,7 @@
         <v>2</v>
       </c>
       <c r="I169" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -5970,7 +5970,7 @@
         <v>11326</v>
       </c>
       <c r="B170" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C170">
         <v>11</v>
@@ -5979,10 +5979,10 @@
         <v>16</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G170" t="s">
         <v>10</v>
@@ -5991,7 +5991,7 @@
         <v>9</v>
       </c>
       <c r="I170" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -5999,7 +5999,7 @@
         <v>11327</v>
       </c>
       <c r="B171" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C171">
         <v>12</v>
@@ -6008,10 +6008,10 @@
         <v>17</v>
       </c>
       <c r="E171" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F171" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="G171" t="s">
         <v>10</v>
@@ -6020,7 +6020,7 @@
         <v>4</v>
       </c>
       <c r="I171" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -6028,7 +6028,7 @@
         <v>11327</v>
       </c>
       <c r="B172" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C172">
         <v>12</v>
@@ -6037,10 +6037,10 @@
         <v>17</v>
       </c>
       <c r="E172" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F172" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F172" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="G172" t="s">
         <v>20</v>
@@ -6049,7 +6049,7 @@
         <v>4</v>
       </c>
       <c r="I172" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -6057,7 +6057,7 @@
         <v>11328</v>
       </c>
       <c r="B173" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C173">
         <v>13</v>
@@ -6066,10 +6066,10 @@
         <v>18</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G173" t="s">
         <v>10</v>
@@ -6078,7 +6078,7 @@
         <v>4</v>
       </c>
       <c r="I173" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -6086,7 +6086,7 @@
         <v>11328</v>
       </c>
       <c r="B174" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C174">
         <v>13</v>
@@ -6095,10 +6095,10 @@
         <v>18</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G174" t="s">
         <v>20</v>
@@ -6107,7 +6107,7 @@
         <v>3</v>
       </c>
       <c r="I174" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -6115,7 +6115,7 @@
         <v>11329</v>
       </c>
       <c r="B175" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C175">
         <v>13</v>
@@ -6124,7 +6124,7 @@
         <v>19</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>24</v>
@@ -6136,7 +6136,7 @@
         <v>4</v>
       </c>
       <c r="I175" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -6144,7 +6144,7 @@
         <v>11329</v>
       </c>
       <c r="B176" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C176">
         <v>13</v>
@@ -6153,7 +6153,7 @@
         <v>19</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>24</v>
@@ -6165,7 +6165,7 @@
         <v>3</v>
       </c>
       <c r="I176" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -6173,7 +6173,7 @@
         <v>11405</v>
       </c>
       <c r="B177" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C177">
         <v>4</v>
@@ -6182,10 +6182,10 @@
         <v>5</v>
       </c>
       <c r="E177" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F177" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="G177" t="s">
         <v>10</v>
@@ -6202,7 +6202,7 @@
         <v>11405</v>
       </c>
       <c r="B178" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C178">
         <v>4</v>
@@ -6211,10 +6211,10 @@
         <v>5</v>
       </c>
       <c r="E178" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F178" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="G178" t="s">
         <v>20</v>
@@ -6231,7 +6231,7 @@
         <v>11406</v>
       </c>
       <c r="B179" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C179">
         <v>4</v>
@@ -6240,10 +6240,10 @@
         <v>6</v>
       </c>
       <c r="E179" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F179" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="F179" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="G179" t="s">
         <v>10</v>
@@ -6252,7 +6252,7 @@
         <v>7</v>
       </c>
       <c r="I179" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
@@ -6260,7 +6260,7 @@
         <v>11406</v>
       </c>
       <c r="B180" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C180">
         <v>4</v>
@@ -6269,10 +6269,10 @@
         <v>6</v>
       </c>
       <c r="E180" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F180" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="F180" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="G180" t="s">
         <v>20</v>
@@ -6281,7 +6281,7 @@
         <v>2</v>
       </c>
       <c r="I180" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -6289,7 +6289,7 @@
         <v>11407</v>
       </c>
       <c r="B181" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C181">
         <v>5</v>
@@ -6298,10 +6298,10 @@
         <v>7</v>
       </c>
       <c r="E181" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F181" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="F181" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="G181" t="s">
         <v>10</v>
@@ -6310,7 +6310,7 @@
         <v>8</v>
       </c>
       <c r="I181" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -6318,7 +6318,7 @@
         <v>11407</v>
       </c>
       <c r="B182" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C182">
         <v>5</v>
@@ -6327,10 +6327,10 @@
         <v>7</v>
       </c>
       <c r="E182" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F182" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="F182" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="G182" t="s">
         <v>11</v>
@@ -6339,7 +6339,7 @@
         <v>2</v>
       </c>
       <c r="I182" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -6347,7 +6347,7 @@
         <v>11408</v>
       </c>
       <c r="B183" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C183">
         <v>6</v>
@@ -6356,10 +6356,10 @@
         <v>8</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G183" t="s">
         <v>10</v>
@@ -6368,7 +6368,7 @@
         <v>8</v>
       </c>
       <c r="I183" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -6376,7 +6376,7 @@
         <v>11408</v>
       </c>
       <c r="B184" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C184">
         <v>6</v>
@@ -6385,10 +6385,10 @@
         <v>8</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G184" t="s">
         <v>20</v>
@@ -6397,7 +6397,7 @@
         <v>3</v>
       </c>
       <c r="I184" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
@@ -6405,7 +6405,7 @@
         <v>11409</v>
       </c>
       <c r="B185" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C185">
         <v>6</v>
@@ -6414,10 +6414,10 @@
         <v>9</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G185" t="s">
         <v>10</v>
@@ -6426,7 +6426,7 @@
         <v>8</v>
       </c>
       <c r="I185" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -6434,7 +6434,7 @@
         <v>11409</v>
       </c>
       <c r="B186" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C186">
         <v>6</v>
@@ -6443,10 +6443,10 @@
         <v>9</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G186" t="s">
         <v>20</v>
@@ -6455,7 +6455,7 @@
         <v>3</v>
       </c>
       <c r="I186" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -6463,7 +6463,7 @@
         <v>11410</v>
       </c>
       <c r="B187" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C187">
         <v>7</v>
@@ -6472,7 +6472,7 @@
         <v>10</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>24</v>
@@ -6484,7 +6484,7 @@
         <v>8</v>
       </c>
       <c r="I187" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
@@ -6492,7 +6492,7 @@
         <v>11410</v>
       </c>
       <c r="B188" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C188">
         <v>7</v>
@@ -6501,7 +6501,7 @@
         <v>10</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>24</v>
@@ -6513,7 +6513,7 @@
         <v>2</v>
       </c>
       <c r="I188" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -6521,7 +6521,7 @@
         <v>11410</v>
       </c>
       <c r="B189" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C189">
         <v>7</v>
@@ -6530,7 +6530,7 @@
         <v>10</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>24</v>
@@ -6542,7 +6542,7 @@
         <v>2</v>
       </c>
       <c r="I189" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
@@ -6550,7 +6550,7 @@
         <v>11506</v>
       </c>
       <c r="B190" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C190">
         <v>4</v>
@@ -6559,10 +6559,10 @@
         <v>6</v>
       </c>
       <c r="E190" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F190" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="F190" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="G190" t="s">
         <v>10</v>
@@ -6579,7 +6579,7 @@
         <v>11506</v>
       </c>
       <c r="B191" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C191">
         <v>4</v>
@@ -6588,10 +6588,10 @@
         <v>6</v>
       </c>
       <c r="E191" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F191" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="F191" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="G191" t="s">
         <v>11</v>
@@ -6608,7 +6608,7 @@
         <v>11507</v>
       </c>
       <c r="B192" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C192">
         <v>5</v>
@@ -6617,10 +6617,10 @@
         <v>7</v>
       </c>
       <c r="E192" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F192" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="F192" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="G192" t="s">
         <v>10</v>
@@ -6629,7 +6629,7 @@
         <v>6</v>
       </c>
       <c r="I192" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -6637,7 +6637,7 @@
         <v>11507</v>
       </c>
       <c r="B193" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C193">
         <v>5</v>
@@ -6646,10 +6646,10 @@
         <v>7</v>
       </c>
       <c r="E193" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F193" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="F193" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="G193" t="s">
         <v>20</v>
@@ -6658,7 +6658,7 @@
         <v>4</v>
       </c>
       <c r="I193" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
@@ -6666,7 +6666,7 @@
         <v>11508</v>
       </c>
       <c r="B194" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C194">
         <v>6</v>
@@ -6675,10 +6675,10 @@
         <v>8</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G194" t="s">
         <v>10</v>
@@ -6687,7 +6687,7 @@
         <v>5</v>
       </c>
       <c r="I194" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
@@ -6695,7 +6695,7 @@
         <v>11508</v>
       </c>
       <c r="B195" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C195">
         <v>6</v>
@@ -6704,10 +6704,10 @@
         <v>8</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G195" t="s">
         <v>20</v>
@@ -6716,7 +6716,7 @@
         <v>4</v>
       </c>
       <c r="I195" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
@@ -6724,7 +6724,7 @@
         <v>11509</v>
       </c>
       <c r="B196" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C196">
         <v>7</v>
@@ -6733,7 +6733,7 @@
         <v>9</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>24</v>
@@ -6745,7 +6745,7 @@
         <v>7</v>
       </c>
       <c r="I196" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
@@ -6753,7 +6753,7 @@
         <v>11509</v>
       </c>
       <c r="B197" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C197">
         <v>7</v>
@@ -6762,7 +6762,7 @@
         <v>9</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>24</v>
@@ -6774,7 +6774,7 @@
         <v>2</v>
       </c>
       <c r="I197" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
@@ -6782,7 +6782,7 @@
         <v>11509</v>
       </c>
       <c r="B198" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C198">
         <v>7</v>
@@ -6791,7 +6791,7 @@
         <v>9</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>24</v>
@@ -6803,7 +6803,7 @@
         <v>1</v>
       </c>
       <c r="I198" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
@@ -6811,7 +6811,7 @@
         <v>11626</v>
       </c>
       <c r="B199" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C199">
         <v>16</v>
@@ -6823,7 +6823,7 @@
         <v>9</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G199" t="s">
         <v>10</v>
@@ -6840,7 +6840,7 @@
         <v>11626</v>
       </c>
       <c r="B200" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C200">
         <v>16</v>
@@ -6852,7 +6852,7 @@
         <v>9</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G200" t="s">
         <v>20</v>
@@ -6869,7 +6869,7 @@
         <v>11627</v>
       </c>
       <c r="B201" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C201">
         <v>17</v>
@@ -6878,10 +6878,10 @@
         <v>27</v>
       </c>
       <c r="E201" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F201" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="F201" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="G201" t="s">
         <v>10</v>
@@ -6890,7 +6890,7 @@
         <v>5</v>
       </c>
       <c r="I201" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
@@ -6898,7 +6898,7 @@
         <v>11627</v>
       </c>
       <c r="B202" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C202">
         <v>17</v>
@@ -6907,10 +6907,10 @@
         <v>27</v>
       </c>
       <c r="E202" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F202" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="F202" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="G202" t="s">
         <v>11</v>
@@ -6919,7 +6919,7 @@
         <v>4</v>
       </c>
       <c r="I202" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
@@ -6927,7 +6927,7 @@
         <v>11628</v>
       </c>
       <c r="B203" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C203">
         <v>18</v>
@@ -6936,10 +6936,10 @@
         <v>28</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G203" t="s">
         <v>20</v>
@@ -6948,7 +6948,7 @@
         <v>5</v>
       </c>
       <c r="I203" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
@@ -6956,7 +6956,7 @@
         <v>11628</v>
       </c>
       <c r="B204" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C204">
         <v>18</v>
@@ -6965,10 +6965,10 @@
         <v>28</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G204" t="s">
         <v>18</v>
@@ -6977,7 +6977,7 @@
         <v>2</v>
       </c>
       <c r="I204" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
@@ -6985,7 +6985,7 @@
         <v>11628</v>
       </c>
       <c r="B205" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C205">
         <v>18</v>
@@ -6994,19 +6994,19 @@
         <v>28</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F205" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G205" t="s">
         <v>218</v>
-      </c>
-      <c r="G205" t="s">
-        <v>219</v>
       </c>
       <c r="H205">
         <v>1</v>
       </c>
       <c r="I205" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
@@ -7014,7 +7014,7 @@
         <v>11629</v>
       </c>
       <c r="B206" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C206">
         <v>19</v>
@@ -7023,7 +7023,7 @@
         <v>29</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>24</v>
@@ -7035,7 +7035,7 @@
         <v>4</v>
       </c>
       <c r="I206" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
@@ -7043,7 +7043,7 @@
         <v>11629</v>
       </c>
       <c r="B207" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C207">
         <v>19</v>
@@ -7052,7 +7052,7 @@
         <v>29</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>24</v>
@@ -7064,7 +7064,7 @@
         <v>2</v>
       </c>
       <c r="I207" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
@@ -7072,7 +7072,7 @@
         <v>11629</v>
       </c>
       <c r="B208" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C208">
         <v>19</v>
@@ -7081,7 +7081,7 @@
         <v>29</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>24</v>
@@ -7093,7 +7093,7 @@
         <v>2</v>
       </c>
       <c r="I208" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -7101,7 +7101,7 @@
         <v>11706</v>
       </c>
       <c r="B209" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C209">
         <v>4</v>
@@ -7110,10 +7110,10 @@
         <v>6</v>
       </c>
       <c r="E209" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F209" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="F209" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="G209" t="s">
         <v>10</v>
@@ -7130,7 +7130,7 @@
         <v>11707</v>
       </c>
       <c r="B210" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C210">
         <v>5</v>
@@ -7139,10 +7139,10 @@
         <v>7</v>
       </c>
       <c r="E210" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F210" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="F210" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="G210" t="s">
         <v>10</v>
@@ -7151,7 +7151,7 @@
         <v>6</v>
       </c>
       <c r="I210" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
@@ -7159,7 +7159,7 @@
         <v>11707</v>
       </c>
       <c r="B211" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C211">
         <v>5</v>
@@ -7168,10 +7168,10 @@
         <v>7</v>
       </c>
       <c r="E211" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F211" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="F211" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="G211" t="s">
         <v>20</v>
@@ -7180,7 +7180,7 @@
         <v>4</v>
       </c>
       <c r="I211" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -7188,7 +7188,7 @@
         <v>11708</v>
       </c>
       <c r="B212" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C212">
         <v>6</v>
@@ -7197,10 +7197,10 @@
         <v>8</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G212" t="s">
         <v>53</v>
@@ -7209,7 +7209,7 @@
         <v>5</v>
       </c>
       <c r="I212" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
@@ -7217,7 +7217,7 @@
         <v>11708</v>
       </c>
       <c r="B213" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C213">
         <v>6</v>
@@ -7226,10 +7226,10 @@
         <v>8</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G213" t="s">
         <v>20</v>
@@ -7238,7 +7238,7 @@
         <v>3</v>
       </c>
       <c r="I213" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -7246,7 +7246,7 @@
         <v>11708</v>
       </c>
       <c r="B214" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C214">
         <v>6</v>
@@ -7255,10 +7255,10 @@
         <v>8</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G214" t="s">
         <v>18</v>
@@ -7267,7 +7267,7 @@
         <v>2</v>
       </c>
       <c r="I214" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
@@ -7275,7 +7275,7 @@
         <v>11709</v>
       </c>
       <c r="B215" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C215">
         <v>7</v>
@@ -7284,10 +7284,10 @@
         <v>9</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G215" t="s">
         <v>11</v>
@@ -7296,7 +7296,7 @@
         <v>1</v>
       </c>
       <c r="I215" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
@@ -7304,7 +7304,7 @@
         <v>11710</v>
       </c>
       <c r="B216" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C216">
         <v>7</v>
@@ -7313,7 +7313,7 @@
         <v>10</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>24</v>
@@ -7325,7 +7325,7 @@
         <v>4</v>
       </c>
       <c r="I216" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
@@ -7333,7 +7333,7 @@
         <v>11710</v>
       </c>
       <c r="B217" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C217">
         <v>7</v>
@@ -7342,7 +7342,7 @@
         <v>10</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>24</v>
@@ -7354,7 +7354,7 @@
         <v>3</v>
       </c>
       <c r="I217" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
@@ -7362,7 +7362,7 @@
         <v>11710</v>
       </c>
       <c r="B218" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C218">
         <v>7</v>
@@ -7371,7 +7371,7 @@
         <v>10</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>24</v>
@@ -7383,7 +7383,7 @@
         <v>2</v>
       </c>
       <c r="I218" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some disprop indices and also now fully report them in codebook
</commit_message>
<xml_diff>
--- a/inst/extdata/additional_govdata.xlsx
+++ b/inst/extdata/additional_govdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\bldrt\bundeslaendeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF20CC5-D9BE-4D8A-8D67-C4A43ED93EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50805598-1A14-47D3-88D5-8BC36C99B419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="246">
   <si>
     <t>gov_id</t>
   </si>
@@ -769,6 +769,9 @@
   </si>
   <si>
     <t>https://de.wikipedia.org/wiki/Kabinett_W%C3%BCst_II</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/Kabinett_G%C3%BCnther_II</t>
   </si>
 </sst>
 </file>
@@ -1088,11 +1091,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I233"/>
+  <dimension ref="A1:I235"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I141" sqref="I141"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I225" sqref="I225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7503,7 +7506,7 @@
         <v>217</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>24</v>
+        <v>243</v>
       </c>
       <c r="G221" t="s">
         <v>10</v>
@@ -7532,7 +7535,7 @@
         <v>217</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>24</v>
+        <v>243</v>
       </c>
       <c r="G222" t="s">
         <v>18</v>
@@ -7561,7 +7564,7 @@
         <v>217</v>
       </c>
       <c r="F223" s="1" t="s">
-        <v>24</v>
+        <v>243</v>
       </c>
       <c r="G223" t="s">
         <v>11</v>
@@ -7575,147 +7578,147 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224">
-        <v>11706</v>
+        <v>11630</v>
       </c>
       <c r="B224" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C224">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D224">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="F224" s="1" t="s">
-        <v>223</v>
+        <v>24</v>
       </c>
       <c r="G224" t="s">
         <v>10</v>
       </c>
       <c r="H224">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I224" t="s">
-        <v>14</v>
+        <v>245</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>11707</v>
+        <v>11630</v>
       </c>
       <c r="B225" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C225">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D225">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="F225" s="1" t="s">
-        <v>224</v>
+        <v>24</v>
       </c>
       <c r="G225" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H225">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I225" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>11707</v>
+        <v>11706</v>
       </c>
       <c r="B226" t="s">
         <v>221</v>
       </c>
       <c r="C226">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D226">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E226" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F226" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F226" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="G226" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H226">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I226" t="s">
-        <v>225</v>
+        <v>14</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>11708</v>
+        <v>11707</v>
       </c>
       <c r="B227" t="s">
         <v>221</v>
       </c>
       <c r="C227">
+        <v>5</v>
+      </c>
+      <c r="D227">
+        <v>7</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G227" t="s">
+        <v>10</v>
+      </c>
+      <c r="H227">
         <v>6</v>
       </c>
-      <c r="D227">
-        <v>8</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F227" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G227" t="s">
-        <v>53</v>
-      </c>
-      <c r="H227">
-        <v>5</v>
-      </c>
       <c r="I227" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>11708</v>
+        <v>11707</v>
       </c>
       <c r="B228" t="s">
         <v>221</v>
       </c>
       <c r="C228">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D228">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E228" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F228" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="F228" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="G228" t="s">
         <v>20</v>
       </c>
       <c r="H228">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I228" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
@@ -7738,10 +7741,10 @@
         <v>226</v>
       </c>
       <c r="G229" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="H229">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I229" t="s">
         <v>227</v>
@@ -7749,57 +7752,57 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230">
-        <v>11709</v>
+        <v>11708</v>
       </c>
       <c r="B230" t="s">
         <v>221</v>
       </c>
       <c r="C230">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D230">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E230" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F230" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="F230" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="G230" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H230">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I230" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231">
-        <v>11710</v>
+        <v>11708</v>
       </c>
       <c r="B231" t="s">
         <v>221</v>
       </c>
       <c r="C231">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D231">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F231" s="1" t="s">
-        <v>24</v>
+        <v>226</v>
       </c>
       <c r="G231" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="H231">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I231" t="s">
         <v>227</v>
@@ -7807,7 +7810,7 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>11710</v>
+        <v>11709</v>
       </c>
       <c r="B232" t="s">
         <v>221</v>
@@ -7816,22 +7819,22 @@
         <v>7</v>
       </c>
       <c r="D232">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E232" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F232" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F232" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G232" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H232">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I232" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
@@ -7854,12 +7857,70 @@
         <v>24</v>
       </c>
       <c r="G233" t="s">
+        <v>53</v>
+      </c>
+      <c r="H233">
+        <v>4</v>
+      </c>
+      <c r="I233" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>11710</v>
+      </c>
+      <c r="B234" t="s">
+        <v>221</v>
+      </c>
+      <c r="C234">
+        <v>7</v>
+      </c>
+      <c r="D234">
+        <v>10</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G234" t="s">
+        <v>20</v>
+      </c>
+      <c r="H234">
+        <v>3</v>
+      </c>
+      <c r="I234" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>11710</v>
+      </c>
+      <c r="B235" t="s">
+        <v>221</v>
+      </c>
+      <c r="C235">
+        <v>7</v>
+      </c>
+      <c r="D235">
+        <v>10</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G235" t="s">
         <v>18</v>
       </c>
-      <c r="H233">
+      <c r="H235">
         <v>2</v>
       </c>
-      <c r="I233" t="s">
+      <c r="I235" t="s">
         <v>227</v>
       </c>
     </row>

</xml_diff>